<commit_message>
Maize transport not working
</commit_message>
<xml_diff>
--- a/keyboards/maize/rgb worksheet.xlsx
+++ b/keyboards/maize/rgb worksheet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaplan/gh/rabbit-88/qmk/keyboards/maize/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC63FA3-445D-AD48-82F1-CD75207ECF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C9607F-A6C3-0240-AF8D-CD35ED5673DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="500" windowWidth="27400" windowHeight="12500" xr2:uid="{EB788031-67B8-8D44-8F7B-6CE0B9408CB8}"/>
+    <workbookView xWindow="7940" yWindow="1540" windowWidth="24900" windowHeight="12320" xr2:uid="{EB788031-67B8-8D44-8F7B-6CE0B9408CB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,7 +54,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -183,39 +183,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -554,7 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DFBA958-0DF9-4349-B04B-20BD84E3F2CD}">
   <dimension ref="A2:AS24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
@@ -1199,56 +1199,56 @@
         <v>0</v>
       </c>
       <c r="B14" s="23">
-        <f>ROUND(B7,0)</f>
+        <f t="shared" ref="B14:C16" si="0">ROUND(B7,0)</f>
         <v>0</v>
       </c>
       <c r="C14" s="23">
-        <f>ROUND(C7,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="23">
-        <f>ROUND(E7,0)</f>
+        <f t="shared" ref="E14:F16" si="1">ROUND(E7,0)</f>
         <v>17</v>
       </c>
       <c r="F14" s="23">
-        <f>ROUND(F7,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G14" s="24"/>
       <c r="H14" s="23">
-        <f>ROUND(H7,0)</f>
+        <f t="shared" ref="H14:I16" si="2">ROUND(H7,0)</f>
         <v>34</v>
       </c>
       <c r="I14" s="23">
-        <f>ROUND(I7,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J14" s="24"/>
       <c r="K14" s="23">
-        <f>ROUND(K7,0)</f>
+        <f t="shared" ref="K14:L16" si="3">ROUND(K7,0)</f>
         <v>52</v>
       </c>
       <c r="L14" s="23">
-        <f>ROUND(L7,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M14" s="24"/>
       <c r="N14" s="23">
-        <f>ROUND(N7,0)</f>
+        <f t="shared" ref="N14:O17" si="4">ROUND(N7,0)</f>
         <v>69</v>
       </c>
       <c r="O14" s="23">
-        <f>ROUND(O7,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P14" s="24"/>
       <c r="Q14" s="23">
-        <f>ROUND(Q7,0)</f>
+        <f t="shared" ref="Q14:R17" si="5">ROUND(Q7,0)</f>
         <v>107</v>
       </c>
       <c r="R14" s="23">
-        <f>ROUND(R7,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S14" s="24"/>
@@ -1259,56 +1259,56 @@
       <c r="X14" s="24"/>
       <c r="Y14" s="24"/>
       <c r="Z14" s="23">
-        <f>ROUND(Z7,0)</f>
+        <f t="shared" ref="Z14:AA17" si="6">ROUND(Z7,0)</f>
         <v>138</v>
       </c>
       <c r="AA14" s="23">
-        <f>ROUND(AA7,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="AB14" s="24"/>
       <c r="AC14" s="23">
-        <f>ROUND(AC7,0)</f>
+        <f t="shared" ref="AC14:AD17" si="7">ROUND(AC7,0)</f>
         <v>155</v>
       </c>
       <c r="AD14" s="23">
-        <f>ROUND(AD7,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AE14" s="24"/>
       <c r="AF14" s="23">
-        <f>ROUND(AF7,0)</f>
+        <f t="shared" ref="AF14:AG16" si="8">ROUND(AF7,0)</f>
         <v>172</v>
       </c>
       <c r="AG14" s="23">
-        <f>ROUND(AG7,0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH14" s="24"/>
       <c r="AI14" s="23">
-        <f>ROUND(AI7,0)</f>
+        <f t="shared" ref="AI14:AJ16" si="9">ROUND(AI7,0)</f>
         <v>190</v>
       </c>
       <c r="AJ14" s="23">
-        <f>ROUND(AJ7,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AK14" s="24"/>
       <c r="AL14" s="23">
-        <f>ROUND(AL7,0)</f>
+        <f t="shared" ref="AL14:AM16" si="10">ROUND(AL7,0)</f>
         <v>207</v>
       </c>
       <c r="AM14" s="23">
-        <f>ROUND(AM7,0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AN14" s="24"/>
       <c r="AO14" s="23">
-        <f>ROUND(AO7,0)</f>
+        <f t="shared" ref="AO14:AP16" si="11">ROUND(AO7,0)</f>
         <v>224</v>
       </c>
       <c r="AP14" s="23">
-        <f>ROUND(AP7,0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -1317,56 +1317,56 @@
         <v>1</v>
       </c>
       <c r="B15" s="23">
-        <f>ROUND(B8,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C15" s="23">
-        <f>ROUND(C8,0)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="23">
-        <f>ROUND(E8,0)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="F15" s="23">
-        <f>ROUND(F8,0)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="G15" s="24"/>
       <c r="H15" s="23">
-        <f>ROUND(H8,0)</f>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="I15" s="23">
-        <f>ROUND(I8,0)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="J15" s="24"/>
       <c r="K15" s="23">
-        <f>ROUND(K8,0)</f>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="L15" s="23">
-        <f>ROUND(L8,0)</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="M15" s="24"/>
       <c r="N15" s="23">
-        <f>ROUND(N8,0)</f>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="O15" s="23">
-        <f>ROUND(O8,0)</f>
+        <f t="shared" si="4"/>
         <v>21</v>
       </c>
       <c r="P15" s="24"/>
       <c r="Q15" s="23">
-        <f>ROUND(Q8,0)</f>
+        <f t="shared" si="5"/>
         <v>107</v>
       </c>
       <c r="R15" s="23">
-        <f>ROUND(R8,0)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="S15" s="24"/>
@@ -1377,56 +1377,56 @@
       <c r="X15" s="24"/>
       <c r="Y15" s="24"/>
       <c r="Z15" s="23">
-        <f>ROUND(Z8,0)</f>
+        <f t="shared" si="6"/>
         <v>138</v>
       </c>
       <c r="AA15" s="23">
-        <f>ROUND(AA8,0)</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="AB15" s="24"/>
       <c r="AC15" s="23">
-        <f>ROUND(AC8,0)</f>
+        <f t="shared" si="7"/>
         <v>155</v>
       </c>
       <c r="AD15" s="23">
-        <f>ROUND(AD8,0)</f>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
       <c r="AE15" s="24"/>
       <c r="AF15" s="23">
-        <f>ROUND(AF8,0)</f>
+        <f t="shared" si="8"/>
         <v>172</v>
       </c>
       <c r="AG15" s="23">
-        <f>ROUND(AG8,0)</f>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="AH15" s="24"/>
       <c r="AI15" s="23">
-        <f>ROUND(AI8,0)</f>
+        <f t="shared" si="9"/>
         <v>190</v>
       </c>
       <c r="AJ15" s="23">
-        <f>ROUND(AJ8,0)</f>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="AK15" s="24"/>
       <c r="AL15" s="23">
-        <f>ROUND(AL8,0)</f>
+        <f t="shared" si="10"/>
         <v>207</v>
       </c>
       <c r="AM15" s="23">
-        <f>ROUND(AM8,0)</f>
+        <f t="shared" si="10"/>
         <v>21</v>
       </c>
       <c r="AN15" s="24"/>
       <c r="AO15" s="23">
-        <f>ROUND(AO8,0)</f>
+        <f t="shared" si="11"/>
         <v>224</v>
       </c>
       <c r="AP15" s="23">
-        <f>ROUND(AP8,0)</f>
+        <f t="shared" si="11"/>
         <v>21</v>
       </c>
     </row>
@@ -1435,56 +1435,56 @@
         <v>2</v>
       </c>
       <c r="B16" s="23">
-        <f>ROUND(B9,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C16" s="23">
-        <f>ROUND(C9,0)</f>
+        <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="D16" s="24"/>
       <c r="E16" s="23">
-        <f>ROUND(E9,0)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="F16" s="23">
-        <f>ROUND(F9,0)</f>
+        <f t="shared" si="1"/>
         <v>43</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="23">
-        <f>ROUND(H9,0)</f>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="I16" s="23">
-        <f>ROUND(I9,0)</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="J16" s="24"/>
       <c r="K16" s="23">
-        <f>ROUND(K9,0)</f>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="L16" s="23">
-        <f>ROUND(L9,0)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="M16" s="24"/>
       <c r="N16" s="23">
-        <f>ROUND(N9,0)</f>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="O16" s="23">
-        <f>ROUND(O9,0)</f>
+        <f t="shared" si="4"/>
         <v>43</v>
       </c>
       <c r="P16" s="24"/>
       <c r="Q16" s="23">
-        <f>ROUND(Q9,0)</f>
+        <f t="shared" si="5"/>
         <v>107</v>
       </c>
       <c r="R16" s="23">
-        <f>ROUND(R9,0)</f>
+        <f t="shared" si="5"/>
         <v>43</v>
       </c>
       <c r="S16" s="24"/>
@@ -1495,56 +1495,56 @@
       <c r="X16" s="25"/>
       <c r="Y16" s="25"/>
       <c r="Z16" s="23">
-        <f>ROUND(Z9,0)</f>
+        <f t="shared" si="6"/>
         <v>138</v>
       </c>
       <c r="AA16" s="23">
-        <f>ROUND(AA9,0)</f>
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
       <c r="AB16" s="24"/>
       <c r="AC16" s="23">
-        <f>ROUND(AC9,0)</f>
+        <f t="shared" si="7"/>
         <v>155</v>
       </c>
       <c r="AD16" s="23">
-        <f>ROUND(AD9,0)</f>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
       <c r="AE16" s="24"/>
       <c r="AF16" s="23">
-        <f>ROUND(AF9,0)</f>
+        <f t="shared" si="8"/>
         <v>172</v>
       </c>
       <c r="AG16" s="23">
-        <f>ROUND(AG9,0)</f>
+        <f t="shared" si="8"/>
         <v>43</v>
       </c>
       <c r="AH16" s="24"/>
       <c r="AI16" s="23">
-        <f>ROUND(AI9,0)</f>
+        <f t="shared" si="9"/>
         <v>190</v>
       </c>
       <c r="AJ16" s="23">
-        <f>ROUND(AJ9,0)</f>
+        <f t="shared" si="9"/>
         <v>43</v>
       </c>
       <c r="AK16" s="24"/>
       <c r="AL16" s="23">
-        <f>ROUND(AL9,0)</f>
+        <f t="shared" si="10"/>
         <v>207</v>
       </c>
       <c r="AM16" s="23">
-        <f>ROUND(AM9,0)</f>
+        <f t="shared" si="10"/>
         <v>43</v>
       </c>
       <c r="AN16" s="24"/>
       <c r="AO16" s="23">
-        <f>ROUND(AO9,0)</f>
+        <f t="shared" si="11"/>
         <v>224</v>
       </c>
       <c r="AP16" s="23">
-        <f>ROUND(AP9,0)</f>
+        <f t="shared" si="11"/>
         <v>43</v>
       </c>
     </row>
@@ -1565,20 +1565,20 @@
       <c r="L17" s="24"/>
       <c r="M17" s="24"/>
       <c r="N17" s="23">
-        <f>ROUND(N10,0)</f>
+        <f t="shared" si="4"/>
         <v>69</v>
       </c>
       <c r="O17" s="23">
-        <f>ROUND(O10,0)</f>
+        <f t="shared" si="4"/>
         <v>64</v>
       </c>
       <c r="P17" s="25"/>
       <c r="Q17" s="23">
-        <f>ROUND(Q10,0)</f>
+        <f t="shared" si="5"/>
         <v>107</v>
       </c>
       <c r="R17" s="23">
-        <f>ROUND(R10,0)</f>
+        <f t="shared" si="5"/>
         <v>64</v>
       </c>
       <c r="S17" s="25"/>
@@ -1601,20 +1601,20 @@
       </c>
       <c r="Y17" s="25"/>
       <c r="Z17" s="23">
-        <f>ROUND(Z10,0)</f>
+        <f t="shared" si="6"/>
         <v>138</v>
       </c>
       <c r="AA17" s="23">
-        <f>ROUND(AA10,0)</f>
+        <f t="shared" si="6"/>
         <v>64</v>
       </c>
       <c r="AB17" s="25"/>
       <c r="AC17" s="23">
-        <f>ROUND(AC10,0)</f>
+        <f t="shared" si="7"/>
         <v>155</v>
       </c>
       <c r="AD17" s="23">
-        <f>ROUND(AD10,0)</f>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
       <c r="AE17" s="25"/>

</xml_diff>